<commit_message>
Ver 1.1, Look like code working proper, just divide code into part , function
</commit_message>
<xml_diff>
--- a/Elephant.xlsx
+++ b/Elephant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\safet\PycharmProjects\Słonie_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B43240-897C-4866-8D95-F549FAD69916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6703C91E-5CAA-4E1C-9FAE-F44CE2B51D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="165" windowWidth="12720" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-150" yWindow="90" windowWidth="8550" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,13 +59,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +99,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="C13:H24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,7 +399,7 @@
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -389,99 +412,115 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>1500</v>
+        <v>2400</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>2000</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1200</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2400</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1600</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>4000</v>
       </c>
-      <c r="C3">
+      <c r="C7">
         <v>2</v>
       </c>
-      <c r="D3">
+      <c r="D7">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>3300</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
+      <c r="E7" s="3"/>
+      <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>2000</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>3200</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>1700</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>500</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>1100</v>
-      </c>
-      <c r="C9">
-        <v>8</v>
-      </c>
-      <c r="D9">
-        <v>5</v>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f>1500+4000+5000+2500+3100+4300</f>
+        <v>20400</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ver 1.2, Everything set, and well commented
</commit_message>
<xml_diff>
--- a/Elephant.xlsx
+++ b/Elephant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\safet\PycharmProjects\Słonie_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6703C91E-5CAA-4E1C-9FAE-F44CE2B51D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8305AC8A-F62E-4B95-9AC6-34A2D5F37D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-150" yWindow="90" windowWidth="8550" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="8550" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,32 +59,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,12 +80,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,7 +365,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,7 +389,6 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -427,7 +403,6 @@
       <c r="D2">
         <v>5</v>
       </c>
-      <c r="E2" s="2"/>
       <c r="F2">
         <v>1</v>
       </c>
@@ -442,7 +417,6 @@
       <c r="D3">
         <v>3</v>
       </c>
-      <c r="E3" s="3"/>
       <c r="F3">
         <v>2</v>
       </c>
@@ -457,7 +431,6 @@
       <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" s="3"/>
       <c r="F4">
         <v>3</v>
       </c>
@@ -472,7 +445,6 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="E5" s="4"/>
       <c r="F5">
         <v>4</v>
       </c>
@@ -487,7 +459,6 @@
       <c r="D6">
         <v>6</v>
       </c>
-      <c r="E6" s="4"/>
       <c r="F6">
         <v>5</v>
       </c>
@@ -502,16 +473,9 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7" s="3"/>
       <c r="F7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G14">

</xml_diff>

<commit_message>
Ver 1.3 Exchange source of data to .txt file add new function to read file and function to convert data as need to proper functionality of program
</commit_message>
<xml_diff>
--- a/Elephant.xlsx
+++ b/Elephant.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\safet\PycharmProjects\Słonie_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8305AC8A-F62E-4B95-9AC6-34A2D5F37D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7705AB8-A773-467D-A0C7-860C8A9B7A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="8550" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -365,7 +365,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ver 1.4 Read file by using fileinput.input() func
</commit_message>
<xml_diff>
--- a/Elephant.xlsx
+++ b/Elephant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\safet\PycharmProjects\Słonie_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7705AB8-A773-467D-A0C7-860C8A9B7A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51863AC-8ED1-4A45-8788-E1CA953E5993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="8550" windowHeight="15195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,7 +365,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,7 +392,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>2400</v>
@@ -475,6 +475,28 @@
       </c>
       <c r="F7">
         <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>2500</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>5000</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>